<commit_message>
VIsion e Use Case Model
06-09-13
</commit_message>
<xml_diff>
--- a/USE-CASE MODEL (e-Book Store).xlsx
+++ b/USE-CASE MODEL (e-Book Store).xlsx
@@ -96,9 +96,6 @@
     <t>Permitir visualização do repositório de e-books da livraria, descrição das obras e acesso limitado ao primeiro capítulo de cada obra selecionada, podendo então a obra ser adquirida ou não, seja ela paga ou gratuita, seja da própria loja ou de autoria de outro usuário.</t>
   </si>
   <si>
-    <t>Permitir e oferecer o recurso para que quaisquer dos livros visualizados pelo usuário possa ser compartilhado através do facebook e twitter, independente de ter sido adquirido, e permitir comentário do usuário a respeito da referida obra neste mesmo compartilhamento (respeitadas e aceitas as políticas de privacidade das respectivas plataformas).</t>
-  </si>
-  <si>
     <t>Compartilhamento</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Na transação de venda/compra de obras de autoria de usuários cadastrados, cobrar 10% de taxa sobre o preço de venda, e repassá-la à e-Book Store, a cada transação efetivada.</t>
   </si>
   <si>
-    <t>Permitir que o comprador visualize online e/ou faça o download da obra adquirida, através de seu histórico de compras ou aquisições gratuitas.</t>
-  </si>
-  <si>
     <t>Oferecer ao usuário, na visualização de estoques (próprios ou da loja), meios distintos de ordenação das obras, a serem redefinidos pelo usuário a qualquer momento. Permitir ordenação por número de compras (ou aquisições gratuitas) por terceiros; por número de avaliações positivas e recomendações compartilhadas quanto à obra; por preço (crescente ou decrescente); por gratuidade ou não da obra.</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>Encaminhar casos omissos ou não solucionados à direção e ao setor jurídico da empresa antes de ser dada qualquer resposta negativa ao cliente.</t>
   </si>
   <si>
-    <t>Fazer o registro e informar ao cliente o número de protocolo, bem como conferir acesso a este e ao histórico de suas reclamações e respectivas gravações até 90 dias anteriores.</t>
-  </si>
-  <si>
     <t>Gestão de Estoque</t>
   </si>
   <si>
@@ -232,6 +223,15 @@
   </si>
   <si>
     <t>(Requisitos funcionais, nomes de casos de uso e atores, diagrama de UC, etc.)</t>
+  </si>
+  <si>
+    <t>Permitir e oferecer o recurso para que quaisquer dos livros visualizados pelo usuário possa ter seu endereço eletrônico compartilhado através do facebook e twitter, independente de ter sido adquirido, e permitir comentário do usuário a respeito da referida obra neste mesmo compartilhamento, a fim de que outras pessoas, ao se interessarem por esta, possam visualizá-la na e-Books Store após devido cadastro (respeitadas e aceitas as políticas de privacidade das respectivas plataformas).</t>
+  </si>
+  <si>
+    <t>Permitir que o comprador visualize online e/ou faça o download da obra adquirida, através de seu histórico de compras e de aquisições gratuitas.</t>
+  </si>
+  <si>
+    <t>Fazer o registro e informar ao cliente o número de protocolo, bem como conferir acesso a este e ao histórico de suas reclamações e respectivas gravações até 90 dias anteriores ao registro do evento.</t>
   </si>
 </sst>
 </file>
@@ -354,6 +354,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -367,9 +370,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,18 +687,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75">
+      <c r="A2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75">
-      <c r="A2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="5"/>
@@ -706,11 +706,11 @@
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="18.75">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" ht="18.75">
       <c r="A5" s="7"/>
@@ -719,7 +719,7 @@
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -754,18 +754,18 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="105">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="135">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="75">
@@ -773,10 +773,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
@@ -784,10 +784,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
@@ -795,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60">
@@ -806,10 +806,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60">
@@ -817,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45">
@@ -828,10 +828,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="120">
@@ -839,10 +839,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -850,10 +850,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45">
@@ -861,10 +861,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45">
@@ -872,10 +872,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45">
@@ -883,10 +883,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
@@ -894,10 +894,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
@@ -905,10 +905,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="75">
@@ -916,10 +916,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45">
@@ -927,10 +927,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60">
@@ -938,10 +938,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -971,7 +971,7 @@
     </row>
     <row r="32" spans="1:4" ht="21">
       <c r="A32" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -979,120 +979,120 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
-      <c r="A42" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>67</v>
+      <c r="A42" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="14"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:5">

</xml_diff>